<commit_message>
send email using list
</commit_message>
<xml_diff>
--- a/q_email_with_html/이메일리스트_with_name_attachment.xlsx
+++ b/q_email_with_html/이메일리스트_with_name_attachment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\python\fastcampus-python-automation\q_email_with_html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E1C38-8732-4105-BFFD-5FFF3B2A6214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E91BA8-B21B-4DBC-888C-0BA76CCD6937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1470" windowWidth="23310" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>받는분</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,14 @@
   </si>
   <si>
     <t>[패스트몰] 2022-09-22 상품발주 확인 요청8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김영환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[패스트몰] 2022-09-22 상품발주 확인 요청9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -447,7 +455,15 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -502,6 +518,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3A7DDB11-8296-49AC-9E04-634559F396E7}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{4E9CA495-F74E-4273-9C28-B0ADB25BD71E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>